<commit_message>
Update result from 001 - 004
</commit_message>
<xml_diff>
--- a/20160420 - 001/6. Logs/logs.xlsx
+++ b/20160420 - 001/6. Logs/logs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="44">
   <si>
     <t>Time</t>
   </si>
@@ -92,6 +92,60 @@
   </si>
   <si>
     <t>20160425_182615</t>
+  </si>
+  <si>
+    <t>20160426_092010</t>
+  </si>
+  <si>
+    <t>2 layers: [10-Sigmoid, 2-Softmax], learning_rate: 0.01, learning_rule: adagrad, n_iterator: 1000</t>
+  </si>
+  <si>
+    <t>20160426_093448</t>
+  </si>
+  <si>
+    <t>20160426_095000</t>
+  </si>
+  <si>
+    <t>20160426_100456</t>
+  </si>
+  <si>
+    <t>20160426_101945</t>
+  </si>
+  <si>
+    <t>20160426_110626</t>
+  </si>
+  <si>
+    <t>2 layers: [10-Sigmoid, 2-Softmax], learning_rate: 0.01, learning_rule: adagrad, n_iterator: 2000</t>
+  </si>
+  <si>
+    <t>20160426_113404</t>
+  </si>
+  <si>
+    <t>20160426_120242</t>
+  </si>
+  <si>
+    <t>20160426_123026</t>
+  </si>
+  <si>
+    <t>20160426_125821</t>
+  </si>
+  <si>
+    <t>20160426_134421</t>
+  </si>
+  <si>
+    <t>2 layers: [10-Sigmoid, 2-Softmax], learning_rate: 0.01, learning_rule: adagrad, n_iterator: 3000</t>
+  </si>
+  <si>
+    <t>20160426_142730</t>
+  </si>
+  <si>
+    <t>20160426_151016</t>
+  </si>
+  <si>
+    <t>20160426_155310</t>
+  </si>
+  <si>
+    <t>20160426_163451</t>
   </si>
 </sst>
 </file>
@@ -423,7 +477,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -847,6 +901,576 @@
         <v>0.61</v>
       </c>
     </row>
+    <row r="12" spans="1:12">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12">
+        <v>0.920792079207921</v>
+      </c>
+      <c r="L12">
+        <v>0.56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" t="s">
+        <v>27</v>
+      </c>
+      <c r="K13">
+        <v>0.920792079207921</v>
+      </c>
+      <c r="L13">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14">
+        <v>0.924092409240924</v>
+      </c>
+      <c r="L14">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15">
+        <v>0.920792079207921</v>
+      </c>
+      <c r="L15">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16">
+        <v>0.917491749174917</v>
+      </c>
+      <c r="L16">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" t="s">
+        <v>33</v>
+      </c>
+      <c r="K17">
+        <v>0.920792079207921</v>
+      </c>
+      <c r="L17">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K18">
+        <v>0.917491749174917</v>
+      </c>
+      <c r="L18">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" t="s">
+        <v>33</v>
+      </c>
+      <c r="K19">
+        <v>0.920792079207921</v>
+      </c>
+      <c r="L19">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" t="s">
+        <v>33</v>
+      </c>
+      <c r="K20">
+        <v>0.914191419141914</v>
+      </c>
+      <c r="L20">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" t="s">
+        <v>33</v>
+      </c>
+      <c r="I21" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" t="s">
+        <v>33</v>
+      </c>
+      <c r="K21">
+        <v>0.920792079207921</v>
+      </c>
+      <c r="L21">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" t="s">
+        <v>39</v>
+      </c>
+      <c r="I22" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" t="s">
+        <v>39</v>
+      </c>
+      <c r="K22">
+        <v>0.910891089108911</v>
+      </c>
+      <c r="L22">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" t="s">
+        <v>39</v>
+      </c>
+      <c r="I23" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" t="s">
+        <v>39</v>
+      </c>
+      <c r="K23">
+        <v>0.910891089108911</v>
+      </c>
+      <c r="L23">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" t="s">
+        <v>39</v>
+      </c>
+      <c r="I24" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" t="s">
+        <v>39</v>
+      </c>
+      <c r="K24">
+        <v>0.917491749174917</v>
+      </c>
+      <c r="L24">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" t="s">
+        <v>39</v>
+      </c>
+      <c r="G25" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" t="s">
+        <v>39</v>
+      </c>
+      <c r="I25" t="s">
+        <v>14</v>
+      </c>
+      <c r="J25" t="s">
+        <v>39</v>
+      </c>
+      <c r="K25">
+        <v>0.917491749174917</v>
+      </c>
+      <c r="L25">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" t="s">
+        <v>39</v>
+      </c>
+      <c r="G26" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" t="s">
+        <v>39</v>
+      </c>
+      <c r="I26" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26" t="s">
+        <v>39</v>
+      </c>
+      <c r="K26">
+        <v>0.917491749174917</v>
+      </c>
+      <c r="L26">
+        <v>0.45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add results 001 - 004
</commit_message>
<xml_diff>
--- a/20160420 - 001/6. Logs/logs.xlsx
+++ b/20160420 - 001/6. Logs/logs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="50">
   <si>
     <t>Time</t>
   </si>
@@ -146,6 +146,24 @@
   </si>
   <si>
     <t>20160426_163451</t>
+  </si>
+  <si>
+    <t>20160427_084257</t>
+  </si>
+  <si>
+    <t>2 layers: [10-Sigmoid, 2-Softmax], learning_rate: 0.01, learning_rule: adagrad, n_iterator: 4000</t>
+  </si>
+  <si>
+    <t>20160427_093849</t>
+  </si>
+  <si>
+    <t>20160427_103549</t>
+  </si>
+  <si>
+    <t>20160427_113405</t>
+  </si>
+  <si>
+    <t>20160427_123124</t>
   </si>
 </sst>
 </file>
@@ -477,7 +495,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1471,6 +1489,196 @@
         <v>0.45</v>
       </c>
     </row>
+    <row r="27" spans="1:12">
+      <c r="A27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" t="s">
+        <v>45</v>
+      </c>
+      <c r="G27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" t="s">
+        <v>45</v>
+      </c>
+      <c r="I27" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" t="s">
+        <v>45</v>
+      </c>
+      <c r="K27">
+        <v>0.910891089108911</v>
+      </c>
+      <c r="L27">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" t="s">
+        <v>45</v>
+      </c>
+      <c r="G28" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" t="s">
+        <v>45</v>
+      </c>
+      <c r="I28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" t="s">
+        <v>45</v>
+      </c>
+      <c r="K28">
+        <v>0.910891089108911</v>
+      </c>
+      <c r="L28">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" t="s">
+        <v>45</v>
+      </c>
+      <c r="G29" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" t="s">
+        <v>45</v>
+      </c>
+      <c r="I29" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" t="s">
+        <v>45</v>
+      </c>
+      <c r="K29">
+        <v>0.904290429042904</v>
+      </c>
+      <c r="L29">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" t="s">
+        <v>45</v>
+      </c>
+      <c r="G30" t="s">
+        <v>14</v>
+      </c>
+      <c r="H30" t="s">
+        <v>45</v>
+      </c>
+      <c r="I30" t="s">
+        <v>14</v>
+      </c>
+      <c r="J30" t="s">
+        <v>45</v>
+      </c>
+      <c r="K30">
+        <v>0.910891089108911</v>
+      </c>
+      <c r="L30">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" t="s">
+        <v>45</v>
+      </c>
+      <c r="G31" t="s">
+        <v>14</v>
+      </c>
+      <c r="H31" t="s">
+        <v>45</v>
+      </c>
+      <c r="I31" t="s">
+        <v>14</v>
+      </c>
+      <c r="J31" t="s">
+        <v>45</v>
+      </c>
+      <c r="K31">
+        <v>0.910891089108911</v>
+      </c>
+      <c r="L31">
+        <v>0.43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>